<commit_message>
Fixed ACTN3 and >100% bug
Bug fix:
• Fixed issue with ACTN3 (and all + strands) not coming out with the right marks
• Fixed bug where a student can recieve over 100% in their assignments

Known bugs:
• Doesn't work on resolutions below 576px

TODO:
• Create About page
• Optimization
</commit_message>
<xml_diff>
--- a/core/data/ACTN3/Benchling_gRNA_Outputs.xlsx
+++ b/core/data/ACTN3/Benchling_gRNA_Outputs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/43306763dd9133c4/Love/Dias-CRISPR/Dry_lab/MarkingSystem/core/data/ACTN3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\OneDrive\_CoreProjects\SciGrade\SciGrade-Development\core\data\ACTN3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_AA06898EF14268F551D11703FDC09D2E15FBDEE5" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{8E3E10A6-AE17-4F87-92B5-EB857B314D99}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="19200" windowHeight="11355" xr2:uid="{BECC4EE9-076E-4C75-B2ED-50548CDD067E}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="19200" windowHeight="11355" xr2:uid="{BECC4EE9-076E-4C75-B2ED-50548CDD067E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="474">
   <si>
     <t>Position</t>
   </si>
@@ -1020,6 +1021,432 @@
   </si>
   <si>
     <t>CTGGGCTACGGCAGCAGGAG</t>
+  </si>
+  <si>
+    <t>GAGATGCTGAGCCAGCGCGA</t>
+  </si>
+  <si>
+    <t>CTACGATT</t>
+  </si>
+  <si>
+    <t>TAGGGATT</t>
+  </si>
+  <si>
+    <t>GCTATGAGGACTGGCTGCTC</t>
+  </si>
+  <si>
+    <t>TCGGA</t>
+  </si>
+  <si>
+    <t>CGGAG</t>
+  </si>
+  <si>
+    <t>GAGAG</t>
+  </si>
+  <si>
+    <t>TCGCTGCAGGCGCCGGATCT</t>
+  </si>
+  <si>
+    <t>CCGAG</t>
+  </si>
+  <si>
+    <t>TGCTGGAGTCGCTGCAGGCG</t>
+  </si>
+  <si>
+    <t>CCGGA</t>
+  </si>
+  <si>
+    <t>TGGAG</t>
+  </si>
+  <si>
+    <t>CGGAACTTCTCAGCCAGGTG</t>
+  </si>
+  <si>
+    <t>CTGGA</t>
+  </si>
+  <si>
+    <t>GCAGCGACTCCAGCACCTGG</t>
+  </si>
+  <si>
+    <t>CTGAG</t>
+  </si>
+  <si>
+    <t>GAGAA</t>
+  </si>
+  <si>
+    <t>CAGAA</t>
+  </si>
+  <si>
+    <t>CGGAA</t>
+  </si>
+  <si>
+    <t>TCGTGCAGGGAGGCCTTCTG</t>
+  </si>
+  <si>
+    <t>CCGGCAGAAGGCCTCCCTGC</t>
+  </si>
+  <si>
+    <t>ACGAA</t>
+  </si>
+  <si>
+    <t>GGGAG</t>
+  </si>
+  <si>
+    <t>AGGGA</t>
+  </si>
+  <si>
+    <t>CAGGG</t>
+  </si>
+  <si>
+    <t>AAGGCCTCCCTGCACGAAGC</t>
+  </si>
+  <si>
+    <t>TCCCTGCACGAAGCCTGGAC</t>
+  </si>
+  <si>
+    <t>CCGGG</t>
+  </si>
+  <si>
+    <t>CGGGG</t>
+  </si>
+  <si>
+    <t>GGGGA</t>
+  </si>
+  <si>
+    <t>GGGAA</t>
+  </si>
+  <si>
+    <t>AAGGA</t>
+  </si>
+  <si>
+    <t>AGGAG</t>
+  </si>
+  <si>
+    <t>GAGGA</t>
+  </si>
+  <si>
+    <t>CTCAGCATCTCCTCCTTTCC</t>
+  </si>
+  <si>
+    <t>CCCGGGGAAAGGAGGAGATG</t>
+  </si>
+  <si>
+    <t>CCGCACCTCCTGTAGCAAAG</t>
+  </si>
+  <si>
+    <t>CCGAA</t>
+  </si>
+  <si>
+    <t>CAGGA</t>
+  </si>
+  <si>
+    <t>TCGGCTTTGCTACAGGAGGT</t>
+  </si>
+  <si>
+    <t>GCGGG</t>
+  </si>
+  <si>
+    <t>GCGGGCGTTGCTGCGGCGCC</t>
+  </si>
+  <si>
+    <t>ACGAG</t>
+  </si>
+  <si>
+    <t>GCTGCGGCGCCACGAGGCCT</t>
+  </si>
+  <si>
+    <t>TTGAG</t>
+  </si>
+  <si>
+    <t>TGGCGGCGCACCAGGACCGC</t>
+  </si>
+  <si>
+    <t>GTGGA</t>
+  </si>
+  <si>
+    <t>TAGTCCAGCTCATTGAGCTC</t>
+  </si>
+  <si>
+    <t>CTGGG</t>
+  </si>
+  <si>
+    <t>CGCGCTGGCCCAGGAGCTCA</t>
+  </si>
+  <si>
+    <t>ATGAG</t>
+  </si>
+  <si>
+    <t>TGGCCCAGGAGCTCAATGAG</t>
+  </si>
+  <si>
+    <t>CCTCGTGGTAGTCCAGCTCA</t>
+  </si>
+  <si>
+    <t>GCTCAATGAGCTGGACTACC</t>
+  </si>
+  <si>
+    <t>ACTACCACGAGGCAGCCTCA</t>
+  </si>
+  <si>
+    <t>GTGAA</t>
+  </si>
+  <si>
+    <t>GGCCTGGCAGCGGCTATTCA</t>
+  </si>
+  <si>
+    <t>TGCCAGGCCATCTGCGATCA</t>
+  </si>
+  <si>
+    <t>GTGGG</t>
+  </si>
+  <si>
+    <t>TGGGA</t>
+  </si>
+  <si>
+    <t>TCTGCGATCAGTGGGACAAC</t>
+  </si>
+  <si>
+    <t>AAGAG</t>
+  </si>
+  <si>
+    <t>GGCACCCTGACCCAGAAGAG</t>
+  </si>
+  <si>
+    <t>CGGGA</t>
+  </si>
+  <si>
+    <t>TCTAGCGCATCCCGCCTCTT</t>
+  </si>
+  <si>
+    <t>TAGAG</t>
+  </si>
+  <si>
+    <t>AAGAGGCGGGATGCGCTAGA</t>
+  </si>
+  <si>
+    <t>GCGGA</t>
+  </si>
+  <si>
+    <t>GGCGGGATGCGCTAGAGCGG</t>
+  </si>
+  <si>
+    <t>ATGGA</t>
+  </si>
+  <si>
+    <t>TAGAGCGGATGGAGAAGCTC</t>
+  </si>
+  <si>
+    <t>AGACCATTGACCGGCTGCAA</t>
+  </si>
+  <si>
+    <t>CTGCAACTGGAGTTTGCCCG</t>
+  </si>
+  <si>
+    <t>TTGTTGAAGGGCGCGGCCCG</t>
+  </si>
+  <si>
+    <t>AAGGG</t>
+  </si>
+  <si>
+    <t>CGGCACCATCCAGCCAGTTG</t>
+  </si>
+  <si>
+    <t>TTGAA</t>
+  </si>
+  <si>
+    <t>CCGCGCCCTTCAACAACTGG</t>
+  </si>
+  <si>
+    <t>ACAACTGGCTGGATGGTGCC</t>
+  </si>
+  <si>
+    <t>ACGTGTGGCTGGTACACTCT</t>
+  </si>
+  <si>
+    <t>CAGAG</t>
+  </si>
+  <si>
+    <t>TCGTGCGCTGTCAGCAGGCT</t>
+  </si>
+  <si>
+    <t>CAGCCTCGGGCAGTGTTGCC</t>
+  </si>
+  <si>
+    <t>TCAGTTCAAGGCAACACTGC</t>
+  </si>
+  <si>
+    <t>GCAACACTGCCCGAGGCTGA</t>
+  </si>
+  <si>
+    <t>CACCTCGCTCTCAGTCAGCC</t>
+  </si>
+  <si>
+    <t>TCGGG</t>
+  </si>
+  <si>
+    <t>CTGCCCGAGGCTGACTGAGA</t>
+  </si>
+  <si>
+    <t>GCGAG</t>
+  </si>
+  <si>
+    <t>ACTGAGAGCGAGGTGCCATC</t>
+  </si>
+  <si>
+    <t>ATGGG</t>
+  </si>
+  <si>
+    <t>TGCCATCATGGGCATCCAGG</t>
+  </si>
+  <si>
+    <t>GTGAG</t>
+  </si>
+  <si>
+    <t>CAGATCTTCTGGATCTCACC</t>
+  </si>
+  <si>
+    <t>CCATACGTCTGGCAGATCTT</t>
+  </si>
+  <si>
+    <t>CCAGAAGATCTGCCAGACGT</t>
+  </si>
+  <si>
+    <t>TGAGGGTGATGTAGGGATTG</t>
+  </si>
+  <si>
+    <t>TAGGG</t>
+  </si>
+  <si>
+    <t>GAGGG</t>
+  </si>
+  <si>
+    <t>TGGTGTTGATGTCCTGCGGG</t>
+  </si>
+  <si>
+    <t>CCACTTGGTGTTGATGTCCT</t>
+  </si>
+  <si>
+    <t>CCGCAGGACATCAACACCAA</t>
+  </si>
+  <si>
+    <t>AACACCAAGTGGGATATGGT</t>
+  </si>
+  <si>
+    <t>TCACAGCTGGGCACCAGCTT</t>
+  </si>
+  <si>
+    <t>CCTGCAGTGTCTGGTCACAG</t>
+  </si>
+  <si>
+    <t>GCTGGCACGGCAGCAGGTAA</t>
+  </si>
+  <si>
+    <t>GCCTGGGCCGCAAACTGTCG</t>
+  </si>
+  <si>
+    <t>CAGGGTCCAATGGCATTGGC</t>
+  </si>
+  <si>
+    <t>TGCGGCCCAGGCCAATGCCA</t>
+  </si>
+  <si>
+    <t>TTGGA</t>
+  </si>
+  <si>
+    <t>CAGGCCAATGCCATTGGACC</t>
+  </si>
+  <si>
+    <t>CCATTGGACCCTGGATCCAG</t>
+  </si>
+  <si>
+    <t>GCGAA</t>
+  </si>
+  <si>
+    <t>GACCCTGGATCCAGGCGAAG</t>
+  </si>
+  <si>
+    <t>CCCACTTCCTCCACCTTCGC</t>
+  </si>
+  <si>
+    <t>AGGAA</t>
+  </si>
+  <si>
+    <t>TCCAGGCGAAGGTGGAGGAA</t>
+  </si>
+  <si>
+    <t>TGGGG</t>
+  </si>
+  <si>
+    <t>CAGCAGGGCTAGCTGGCTCT</t>
+  </si>
+  <si>
+    <t>CTCTCTGGAGGAGCAGATGG</t>
+  </si>
+  <si>
+    <t>CCGGAT</t>
+  </si>
+  <si>
+    <t>TGGAGT</t>
+  </si>
+  <si>
+    <t>CCGGGT</t>
+  </si>
+  <si>
+    <t>CCGAAT</t>
+  </si>
+  <si>
+    <t>GTGAAT</t>
+  </si>
+  <si>
+    <t>CAGGGT</t>
+  </si>
+  <si>
+    <t>CGGGAT</t>
+  </si>
+  <si>
+    <t>CTGGGT</t>
+  </si>
+  <si>
+    <t>GCGGAT</t>
+  </si>
+  <si>
+    <t>CTGGAT</t>
+  </si>
+  <si>
+    <t>CAGAGT</t>
+  </si>
+  <si>
+    <t>AGGGAT</t>
+  </si>
+  <si>
+    <t>GAGGGT</t>
+  </si>
+  <si>
+    <t>TGGGAT</t>
+  </si>
+  <si>
+    <t>TTTC</t>
+  </si>
+  <si>
+    <t>CTACAGGAGGTGCGGGCGTT</t>
+  </si>
+  <si>
+    <t>TTTG</t>
+  </si>
+  <si>
+    <t>CCCGGCGGGCCGCGCCCTTC</t>
+  </si>
+  <si>
+    <t>GGACCATATCCCACTTGGTG</t>
+  </si>
+  <si>
+    <t>CCTGCTGCCGTGCCAGCTCC</t>
+  </si>
+  <si>
+    <t>TTTA</t>
+  </si>
+  <si>
+    <t>CGGCCCAGGCCAATGCCATT</t>
   </si>
 </sst>
 </file>
@@ -1371,10 +1798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA13F27-6E03-4713-BF80-7B3A8C21CC72}">
-  <dimension ref="A1:F319"/>
+  <dimension ref="A1:F490"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7756,6 +8183,3405 @@
         <v>6.5154925906189201</v>
       </c>
     </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>139</v>
+      </c>
+      <c r="B320">
+        <v>1</v>
+      </c>
+      <c r="C320" t="s">
+        <v>332</v>
+      </c>
+      <c r="D320" t="s">
+        <v>333</v>
+      </c>
+      <c r="E320">
+        <v>49.976927000000003</v>
+      </c>
+      <c r="F320">
+        <v>49.859403620563903</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>658</v>
+      </c>
+      <c r="B321">
+        <v>-1</v>
+      </c>
+      <c r="C321" t="s">
+        <v>288</v>
+      </c>
+      <c r="D321" t="s">
+        <v>334</v>
+      </c>
+      <c r="E321">
+        <v>49.794045400000002</v>
+      </c>
+      <c r="F321">
+        <v>4.1485549768518499</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>26</v>
+      </c>
+      <c r="B322">
+        <v>1</v>
+      </c>
+      <c r="C322" t="s">
+        <v>335</v>
+      </c>
+      <c r="D322" t="s">
+        <v>336</v>
+      </c>
+      <c r="E322">
+        <v>41.253260900000001</v>
+      </c>
+      <c r="F322">
+        <v>1.0658618993601301</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>27</v>
+      </c>
+      <c r="B323">
+        <v>1</v>
+      </c>
+      <c r="C323" t="s">
+        <v>6</v>
+      </c>
+      <c r="D323" t="s">
+        <v>337</v>
+      </c>
+      <c r="E323">
+        <v>40.483896199999997</v>
+      </c>
+      <c r="F323">
+        <v>11.155865334130301</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>34</v>
+      </c>
+      <c r="B324">
+        <v>-1</v>
+      </c>
+      <c r="C324" t="s">
+        <v>187</v>
+      </c>
+      <c r="D324" t="s">
+        <v>338</v>
+      </c>
+      <c r="E324">
+        <v>46.004771400000003</v>
+      </c>
+      <c r="F324">
+        <v>1.2346411905936301</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>36</v>
+      </c>
+      <c r="B325">
+        <v>-1</v>
+      </c>
+      <c r="C325" t="s">
+        <v>339</v>
+      </c>
+      <c r="D325" t="s">
+        <v>340</v>
+      </c>
+      <c r="E325">
+        <v>47.717801999999999</v>
+      </c>
+      <c r="F325">
+        <v>0.27787222477141099</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>44</v>
+      </c>
+      <c r="B326">
+        <v>-1</v>
+      </c>
+      <c r="C326" t="s">
+        <v>341</v>
+      </c>
+      <c r="D326" t="s">
+        <v>342</v>
+      </c>
+      <c r="E326">
+        <v>41.2558705</v>
+      </c>
+      <c r="F326">
+        <v>7.03561876758664</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>61</v>
+      </c>
+      <c r="B327">
+        <v>-1</v>
+      </c>
+      <c r="C327" t="s">
+        <v>14</v>
+      </c>
+      <c r="D327" t="s">
+        <v>343</v>
+      </c>
+      <c r="E327">
+        <v>41.119681399999997</v>
+      </c>
+      <c r="F327">
+        <v>16.570492504943498</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>62</v>
+      </c>
+      <c r="B328">
+        <v>-1</v>
+      </c>
+      <c r="C328" t="s">
+        <v>344</v>
+      </c>
+      <c r="D328" t="s">
+        <v>345</v>
+      </c>
+      <c r="E328">
+        <v>43.355787399999997</v>
+      </c>
+      <c r="F328">
+        <v>15.181430440946</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>63</v>
+      </c>
+      <c r="B329">
+        <v>1</v>
+      </c>
+      <c r="C329" t="s">
+        <v>346</v>
+      </c>
+      <c r="D329" t="s">
+        <v>347</v>
+      </c>
+      <c r="E329">
+        <v>39.618441599999997</v>
+      </c>
+      <c r="F329">
+        <v>81.678283673179806</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>65</v>
+      </c>
+      <c r="B330">
+        <v>1</v>
+      </c>
+      <c r="C330" t="s">
+        <v>192</v>
+      </c>
+      <c r="D330" t="s">
+        <v>348</v>
+      </c>
+      <c r="E330">
+        <v>38.988957200000002</v>
+      </c>
+      <c r="F330">
+        <v>5.1029117725878796</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>77</v>
+      </c>
+      <c r="B331">
+        <v>1</v>
+      </c>
+      <c r="C331" t="s">
+        <v>197</v>
+      </c>
+      <c r="D331" t="s">
+        <v>349</v>
+      </c>
+      <c r="E331">
+        <v>22.765104900000001</v>
+      </c>
+      <c r="F331">
+        <v>54.231835855298897</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>82</v>
+      </c>
+      <c r="B332">
+        <v>-1</v>
+      </c>
+      <c r="C332" t="s">
+        <v>18</v>
+      </c>
+      <c r="D332" t="s">
+        <v>350</v>
+      </c>
+      <c r="E332">
+        <v>38.979161599999998</v>
+      </c>
+      <c r="F332">
+        <v>4.6598857830944702</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>83</v>
+      </c>
+      <c r="B333">
+        <v>-1</v>
+      </c>
+      <c r="C333" t="s">
+        <v>351</v>
+      </c>
+      <c r="D333" t="s">
+        <v>342</v>
+      </c>
+      <c r="E333">
+        <v>38.958379000000001</v>
+      </c>
+      <c r="F333">
+        <v>3.17372763206254</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>93</v>
+      </c>
+      <c r="B334">
+        <v>1</v>
+      </c>
+      <c r="C334" t="s">
+        <v>352</v>
+      </c>
+      <c r="D334" t="s">
+        <v>353</v>
+      </c>
+      <c r="E334">
+        <v>40.363964099999997</v>
+      </c>
+      <c r="F334">
+        <v>2.7476299745176802</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>96</v>
+      </c>
+      <c r="B335">
+        <v>-1</v>
+      </c>
+      <c r="C335" t="s">
+        <v>20</v>
+      </c>
+      <c r="D335" t="s">
+        <v>354</v>
+      </c>
+      <c r="E335">
+        <v>47.410792499999999</v>
+      </c>
+      <c r="F335">
+        <v>14.4058283673454</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>97</v>
+      </c>
+      <c r="B336">
+        <v>-1</v>
+      </c>
+      <c r="C336" t="s">
+        <v>22</v>
+      </c>
+      <c r="D336" t="s">
+        <v>355</v>
+      </c>
+      <c r="E336">
+        <v>46.940170600000002</v>
+      </c>
+      <c r="F336">
+        <v>9.0169063226381301</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>98</v>
+      </c>
+      <c r="B337">
+        <v>-1</v>
+      </c>
+      <c r="C337" t="s">
+        <v>201</v>
+      </c>
+      <c r="D337" t="s">
+        <v>356</v>
+      </c>
+      <c r="E337">
+        <v>46.469295199999998</v>
+      </c>
+      <c r="F337">
+        <v>14.8807662522904</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>100</v>
+      </c>
+      <c r="B338">
+        <v>1</v>
+      </c>
+      <c r="C338" t="s">
+        <v>357</v>
+      </c>
+      <c r="D338" t="s">
+        <v>345</v>
+      </c>
+      <c r="E338">
+        <v>47.429421400000003</v>
+      </c>
+      <c r="F338">
+        <v>3.6398846262666402</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>106</v>
+      </c>
+      <c r="B339">
+        <v>1</v>
+      </c>
+      <c r="C339" t="s">
+        <v>358</v>
+      </c>
+      <c r="D339" t="s">
+        <v>359</v>
+      </c>
+      <c r="E339">
+        <v>41.436056600000001</v>
+      </c>
+      <c r="F339">
+        <v>2.83372969644063</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>107</v>
+      </c>
+      <c r="B340">
+        <v>1</v>
+      </c>
+      <c r="C340" t="s">
+        <v>24</v>
+      </c>
+      <c r="D340" t="s">
+        <v>360</v>
+      </c>
+      <c r="E340">
+        <v>42.2376516</v>
+      </c>
+      <c r="F340">
+        <v>5.3914964533510696</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>108</v>
+      </c>
+      <c r="B341">
+        <v>1</v>
+      </c>
+      <c r="C341" t="s">
+        <v>25</v>
+      </c>
+      <c r="D341" t="s">
+        <v>361</v>
+      </c>
+      <c r="E341">
+        <v>76.534427100000002</v>
+      </c>
+      <c r="F341">
+        <v>8.2018511017979208</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>109</v>
+      </c>
+      <c r="B342">
+        <v>1</v>
+      </c>
+      <c r="C342" t="s">
+        <v>27</v>
+      </c>
+      <c r="D342" t="s">
+        <v>362</v>
+      </c>
+      <c r="E342">
+        <v>84.043192700000006</v>
+      </c>
+      <c r="F342">
+        <v>11.7991866863794</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>113</v>
+      </c>
+      <c r="B343">
+        <v>1</v>
+      </c>
+      <c r="C343" t="s">
+        <v>203</v>
+      </c>
+      <c r="D343" t="s">
+        <v>363</v>
+      </c>
+      <c r="E343">
+        <v>80.372393299999999</v>
+      </c>
+      <c r="F343">
+        <v>5.6020489668515001</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>114</v>
+      </c>
+      <c r="B344">
+        <v>1</v>
+      </c>
+      <c r="C344" t="s">
+        <v>28</v>
+      </c>
+      <c r="D344" t="s">
+        <v>364</v>
+      </c>
+      <c r="E344">
+        <v>80.569716499999998</v>
+      </c>
+      <c r="F344">
+        <v>5.4376992245609799</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>116</v>
+      </c>
+      <c r="B345">
+        <v>1</v>
+      </c>
+      <c r="C345" t="s">
+        <v>204</v>
+      </c>
+      <c r="D345" t="s">
+        <v>365</v>
+      </c>
+      <c r="E345">
+        <v>66.403587999999999</v>
+      </c>
+      <c r="F345">
+        <v>10.1447646938618</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>116</v>
+      </c>
+      <c r="B346">
+        <v>-1</v>
+      </c>
+      <c r="C346" t="s">
+        <v>366</v>
+      </c>
+      <c r="D346" t="s">
+        <v>359</v>
+      </c>
+      <c r="E346">
+        <v>54.2540993</v>
+      </c>
+      <c r="F346">
+        <v>1.82591648618067</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>117</v>
+      </c>
+      <c r="B347">
+        <v>1</v>
+      </c>
+      <c r="C347" t="s">
+        <v>31</v>
+      </c>
+      <c r="D347" t="s">
+        <v>364</v>
+      </c>
+      <c r="E347">
+        <v>54.442358800000001</v>
+      </c>
+      <c r="F347">
+        <v>11.7208247094228</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>125</v>
+      </c>
+      <c r="B348">
+        <v>1</v>
+      </c>
+      <c r="C348" t="s">
+        <v>367</v>
+      </c>
+      <c r="D348" t="s">
+        <v>347</v>
+      </c>
+      <c r="E348">
+        <v>40.672811600000003</v>
+      </c>
+      <c r="F348">
+        <v>5.54322704777283</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>156</v>
+      </c>
+      <c r="B349">
+        <v>-1</v>
+      </c>
+      <c r="C349" t="s">
+        <v>368</v>
+      </c>
+      <c r="D349" t="s">
+        <v>369</v>
+      </c>
+      <c r="E349">
+        <v>45.188416199999999</v>
+      </c>
+      <c r="F349">
+        <v>67.486109203991106</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>158</v>
+      </c>
+      <c r="B350">
+        <v>1</v>
+      </c>
+      <c r="C350" t="s">
+        <v>210</v>
+      </c>
+      <c r="D350" t="s">
+        <v>370</v>
+      </c>
+      <c r="E350">
+        <v>48.376742399999998</v>
+      </c>
+      <c r="F350">
+        <v>25.495984577606301</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>159</v>
+      </c>
+      <c r="B351">
+        <v>1</v>
+      </c>
+      <c r="C351" t="s">
+        <v>34</v>
+      </c>
+      <c r="D351" t="s">
+        <v>364</v>
+      </c>
+      <c r="E351">
+        <v>48.6637944</v>
+      </c>
+      <c r="F351">
+        <v>31.942000751538501</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>166</v>
+      </c>
+      <c r="B352">
+        <v>1</v>
+      </c>
+      <c r="C352" t="s">
+        <v>371</v>
+      </c>
+      <c r="D352" t="s">
+        <v>372</v>
+      </c>
+      <c r="E352">
+        <v>44.960597200000002</v>
+      </c>
+      <c r="F352">
+        <v>5.4289728923337899</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>186</v>
+      </c>
+      <c r="B353">
+        <v>1</v>
+      </c>
+      <c r="C353" t="s">
+        <v>373</v>
+      </c>
+      <c r="D353" t="s">
+        <v>374</v>
+      </c>
+      <c r="E353">
+        <v>44.558717299999998</v>
+      </c>
+      <c r="F353">
+        <v>0.63773616990672899</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>195</v>
+      </c>
+      <c r="B354">
+        <v>1</v>
+      </c>
+      <c r="C354" t="s">
+        <v>375</v>
+      </c>
+      <c r="D354" t="s">
+        <v>376</v>
+      </c>
+      <c r="E354">
+        <v>45.736689699999999</v>
+      </c>
+      <c r="F354">
+        <v>12.780932824874901</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>197</v>
+      </c>
+      <c r="B355">
+        <v>1</v>
+      </c>
+      <c r="C355" t="s">
+        <v>216</v>
+      </c>
+      <c r="D355" t="s">
+        <v>338</v>
+      </c>
+      <c r="E355">
+        <v>48.266843199999997</v>
+      </c>
+      <c r="F355">
+        <v>7.1251429814981204</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>218</v>
+      </c>
+      <c r="B356">
+        <v>1</v>
+      </c>
+      <c r="C356" t="s">
+        <v>220</v>
+      </c>
+      <c r="D356" t="s">
+        <v>370</v>
+      </c>
+      <c r="E356">
+        <v>42.271685300000001</v>
+      </c>
+      <c r="F356">
+        <v>14.7670035405015</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>227</v>
+      </c>
+      <c r="B357">
+        <v>1</v>
+      </c>
+      <c r="C357" t="s">
+        <v>377</v>
+      </c>
+      <c r="D357" t="s">
+        <v>378</v>
+      </c>
+      <c r="E357">
+        <v>24.040192600000001</v>
+      </c>
+      <c r="F357">
+        <v>7.1873701378588999</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>228</v>
+      </c>
+      <c r="B358">
+        <v>1</v>
+      </c>
+      <c r="C358" t="s">
+        <v>47</v>
+      </c>
+      <c r="D358" t="s">
+        <v>343</v>
+      </c>
+      <c r="E358">
+        <v>23.947238899999999</v>
+      </c>
+      <c r="F358">
+        <v>62.425835728126799</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>251</v>
+      </c>
+      <c r="B359">
+        <v>1</v>
+      </c>
+      <c r="C359" t="s">
+        <v>222</v>
+      </c>
+      <c r="D359" t="s">
+        <v>370</v>
+      </c>
+      <c r="E359">
+        <v>47.703066300000003</v>
+      </c>
+      <c r="F359">
+        <v>2.3557832244494601</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>252</v>
+      </c>
+      <c r="B360">
+        <v>1</v>
+      </c>
+      <c r="C360" t="s">
+        <v>51</v>
+      </c>
+      <c r="D360" t="s">
+        <v>364</v>
+      </c>
+      <c r="E360">
+        <v>45.869146200000003</v>
+      </c>
+      <c r="F360">
+        <v>17.988075813946999</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>260</v>
+      </c>
+      <c r="B361">
+        <v>-1</v>
+      </c>
+      <c r="C361" t="s">
+        <v>379</v>
+      </c>
+      <c r="D361" t="s">
+        <v>380</v>
+      </c>
+      <c r="E361">
+        <v>79.103321399999999</v>
+      </c>
+      <c r="F361">
+        <v>22.8467771169489</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>261</v>
+      </c>
+      <c r="B362">
+        <v>1</v>
+      </c>
+      <c r="C362" t="s">
+        <v>381</v>
+      </c>
+      <c r="D362" t="s">
+        <v>382</v>
+      </c>
+      <c r="E362">
+        <v>60.161652099999998</v>
+      </c>
+      <c r="F362">
+        <v>1.3611606867231001</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>266</v>
+      </c>
+      <c r="B363">
+        <v>1</v>
+      </c>
+      <c r="C363" t="s">
+        <v>383</v>
+      </c>
+      <c r="D363" t="s">
+        <v>345</v>
+      </c>
+      <c r="E363">
+        <v>69.4824907</v>
+      </c>
+      <c r="F363">
+        <v>9.9841768755532403</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>268</v>
+      </c>
+      <c r="B364">
+        <v>-1</v>
+      </c>
+      <c r="C364" t="s">
+        <v>384</v>
+      </c>
+      <c r="D364" t="s">
+        <v>376</v>
+      </c>
+      <c r="E364">
+        <v>45.399035699999999</v>
+      </c>
+      <c r="F364">
+        <v>7.98132373531831</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>276</v>
+      </c>
+      <c r="B365">
+        <v>1</v>
+      </c>
+      <c r="C365" t="s">
+        <v>385</v>
+      </c>
+      <c r="D365" t="s">
+        <v>374</v>
+      </c>
+      <c r="E365">
+        <v>90.801578000000006</v>
+      </c>
+      <c r="F365">
+        <v>11.702229798976299</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>290</v>
+      </c>
+      <c r="B366">
+        <v>1</v>
+      </c>
+      <c r="C366" t="s">
+        <v>386</v>
+      </c>
+      <c r="D366" t="s">
+        <v>387</v>
+      </c>
+      <c r="E366">
+        <v>45.078523400000002</v>
+      </c>
+      <c r="F366">
+        <v>54.976586001604403</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>297</v>
+      </c>
+      <c r="B367">
+        <v>-1</v>
+      </c>
+      <c r="C367" t="s">
+        <v>388</v>
+      </c>
+      <c r="D367" t="s">
+        <v>347</v>
+      </c>
+      <c r="E367">
+        <v>47.503847499999999</v>
+      </c>
+      <c r="F367">
+        <v>2.3129796342106701</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>322</v>
+      </c>
+      <c r="B368">
+        <v>1</v>
+      </c>
+      <c r="C368" t="s">
+        <v>389</v>
+      </c>
+      <c r="D368" t="s">
+        <v>390</v>
+      </c>
+      <c r="E368">
+        <v>46.955852100000001</v>
+      </c>
+      <c r="F368">
+        <v>0.90309905049902695</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>323</v>
+      </c>
+      <c r="B369">
+        <v>1</v>
+      </c>
+      <c r="C369" t="s">
+        <v>62</v>
+      </c>
+      <c r="D369" t="s">
+        <v>391</v>
+      </c>
+      <c r="E369">
+        <v>47.931781000000001</v>
+      </c>
+      <c r="F369">
+        <v>14.069324528053199</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>332</v>
+      </c>
+      <c r="B370">
+        <v>1</v>
+      </c>
+      <c r="C370" t="s">
+        <v>392</v>
+      </c>
+      <c r="D370" t="s">
+        <v>380</v>
+      </c>
+      <c r="E370">
+        <v>45.827204899999998</v>
+      </c>
+      <c r="F370">
+        <v>22.8103498302576</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>347</v>
+      </c>
+      <c r="B371">
+        <v>1</v>
+      </c>
+      <c r="C371" t="s">
+        <v>239</v>
+      </c>
+      <c r="D371" t="s">
+        <v>349</v>
+      </c>
+      <c r="E371">
+        <v>43.031854799999998</v>
+      </c>
+      <c r="F371">
+        <v>1.56348313562459</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>350</v>
+      </c>
+      <c r="B372">
+        <v>1</v>
+      </c>
+      <c r="C372" t="s">
+        <v>240</v>
+      </c>
+      <c r="D372" t="s">
+        <v>393</v>
+      </c>
+      <c r="E372">
+        <v>37.944099700000002</v>
+      </c>
+      <c r="F372">
+        <v>22.6660094538347</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>350</v>
+      </c>
+      <c r="B373">
+        <v>-1</v>
+      </c>
+      <c r="C373" t="s">
+        <v>241</v>
+      </c>
+      <c r="D373" t="s">
+        <v>356</v>
+      </c>
+      <c r="E373">
+        <v>44.425019300000002</v>
+      </c>
+      <c r="F373">
+        <v>16.613114018256599</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>355</v>
+      </c>
+      <c r="B374">
+        <v>1</v>
+      </c>
+      <c r="C374" t="s">
+        <v>394</v>
+      </c>
+      <c r="D374" t="s">
+        <v>372</v>
+      </c>
+      <c r="E374">
+        <v>40.259539500000002</v>
+      </c>
+      <c r="F374">
+        <v>28.084197770568199</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>356</v>
+      </c>
+      <c r="B375">
+        <v>1</v>
+      </c>
+      <c r="C375" t="s">
+        <v>72</v>
+      </c>
+      <c r="D375" t="s">
+        <v>395</v>
+      </c>
+      <c r="E375">
+        <v>37.103979199999998</v>
+      </c>
+      <c r="F375">
+        <v>49.076943134890001</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>356</v>
+      </c>
+      <c r="B376">
+        <v>-1</v>
+      </c>
+      <c r="C376" t="s">
+        <v>396</v>
+      </c>
+      <c r="D376" t="s">
+        <v>380</v>
+      </c>
+      <c r="E376">
+        <v>96.029895400000001</v>
+      </c>
+      <c r="F376">
+        <v>5.89317389925833</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>366</v>
+      </c>
+      <c r="B377">
+        <v>1</v>
+      </c>
+      <c r="C377" t="s">
+        <v>243</v>
+      </c>
+      <c r="D377" t="s">
+        <v>397</v>
+      </c>
+      <c r="E377">
+        <v>88.013261499999999</v>
+      </c>
+      <c r="F377">
+        <v>1.91925968363948</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>370</v>
+      </c>
+      <c r="B378">
+        <v>1</v>
+      </c>
+      <c r="C378" t="s">
+        <v>398</v>
+      </c>
+      <c r="D378" t="s">
+        <v>399</v>
+      </c>
+      <c r="E378">
+        <v>94.668598000000003</v>
+      </c>
+      <c r="F378">
+        <v>8.6555626656087892</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>374</v>
+      </c>
+      <c r="B379">
+        <v>1</v>
+      </c>
+      <c r="C379" t="s">
+        <v>400</v>
+      </c>
+      <c r="D379" t="s">
+        <v>401</v>
+      </c>
+      <c r="E379">
+        <v>95.088178799999994</v>
+      </c>
+      <c r="F379">
+        <v>37.451722617105098</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>375</v>
+      </c>
+      <c r="B380">
+        <v>1</v>
+      </c>
+      <c r="C380" t="s">
+        <v>75</v>
+      </c>
+      <c r="D380" t="s">
+        <v>343</v>
+      </c>
+      <c r="E380">
+        <v>92.8072856</v>
+      </c>
+      <c r="F380">
+        <v>6.7132426560464502</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>377</v>
+      </c>
+      <c r="B381">
+        <v>1</v>
+      </c>
+      <c r="C381" t="s">
+        <v>246</v>
+      </c>
+      <c r="D381" t="s">
+        <v>348</v>
+      </c>
+      <c r="E381">
+        <v>91.549823799999999</v>
+      </c>
+      <c r="F381">
+        <v>7.4867514962310198</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>386</v>
+      </c>
+      <c r="B382">
+        <v>1</v>
+      </c>
+      <c r="C382" t="s">
+        <v>402</v>
+      </c>
+      <c r="D382" t="s">
+        <v>345</v>
+      </c>
+      <c r="E382">
+        <v>73.670552599999994</v>
+      </c>
+      <c r="F382">
+        <v>15.287159011330999</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>387</v>
+      </c>
+      <c r="B383">
+        <v>1</v>
+      </c>
+      <c r="C383" t="s">
+        <v>76</v>
+      </c>
+      <c r="D383" t="s">
+        <v>343</v>
+      </c>
+      <c r="E383">
+        <v>66.169603499999994</v>
+      </c>
+      <c r="F383">
+        <v>3.6268349453720301</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>394</v>
+      </c>
+      <c r="B384">
+        <v>-1</v>
+      </c>
+      <c r="C384" t="s">
+        <v>77</v>
+      </c>
+      <c r="D384" t="s">
+        <v>364</v>
+      </c>
+      <c r="E384">
+        <v>47.713571999999999</v>
+      </c>
+      <c r="F384">
+        <v>1.94063884680827</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>395</v>
+      </c>
+      <c r="B385">
+        <v>-1</v>
+      </c>
+      <c r="C385" t="s">
+        <v>250</v>
+      </c>
+      <c r="D385" t="s">
+        <v>370</v>
+      </c>
+      <c r="E385">
+        <v>46.879180099999999</v>
+      </c>
+      <c r="F385">
+        <v>1.0745970249648999</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>410</v>
+      </c>
+      <c r="B386">
+        <v>1</v>
+      </c>
+      <c r="C386" t="s">
+        <v>403</v>
+      </c>
+      <c r="D386" t="s">
+        <v>345</v>
+      </c>
+      <c r="E386">
+        <v>48.481602899999999</v>
+      </c>
+      <c r="F386">
+        <v>25.696284265872102</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>411</v>
+      </c>
+      <c r="B387">
+        <v>1</v>
+      </c>
+      <c r="C387" t="s">
+        <v>81</v>
+      </c>
+      <c r="D387" t="s">
+        <v>343</v>
+      </c>
+      <c r="E387">
+        <v>48.848190700000004</v>
+      </c>
+      <c r="F387">
+        <v>6.0554803872304097</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>424</v>
+      </c>
+      <c r="B388">
+        <v>1</v>
+      </c>
+      <c r="C388" t="s">
+        <v>404</v>
+      </c>
+      <c r="D388" t="s">
+        <v>372</v>
+      </c>
+      <c r="E388">
+        <v>47.9240353</v>
+      </c>
+      <c r="F388">
+        <v>56.724106469670197</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>431</v>
+      </c>
+      <c r="B389">
+        <v>-1</v>
+      </c>
+      <c r="C389" t="s">
+        <v>405</v>
+      </c>
+      <c r="D389" t="s">
+        <v>359</v>
+      </c>
+      <c r="E389">
+        <v>48.448595099999999</v>
+      </c>
+      <c r="F389">
+        <v>7.4521727367436101</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>445</v>
+      </c>
+      <c r="B390">
+        <v>-1</v>
+      </c>
+      <c r="C390" t="s">
+        <v>254</v>
+      </c>
+      <c r="D390" t="s">
+        <v>406</v>
+      </c>
+      <c r="E390">
+        <v>44.386972399999998</v>
+      </c>
+      <c r="F390">
+        <v>2.5022238562400601</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>448</v>
+      </c>
+      <c r="B391">
+        <v>-1</v>
+      </c>
+      <c r="C391" t="s">
+        <v>407</v>
+      </c>
+      <c r="D391" t="s">
+        <v>408</v>
+      </c>
+      <c r="E391">
+        <v>44.1786356</v>
+      </c>
+      <c r="F391">
+        <v>10.474801100437899</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>449</v>
+      </c>
+      <c r="B392">
+        <v>1</v>
+      </c>
+      <c r="C392" t="s">
+        <v>409</v>
+      </c>
+      <c r="D392" t="s">
+        <v>345</v>
+      </c>
+      <c r="E392">
+        <v>44.7592894</v>
+      </c>
+      <c r="F392">
+        <v>25.1359953446722</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>461</v>
+      </c>
+      <c r="B393">
+        <v>1</v>
+      </c>
+      <c r="C393" t="s">
+        <v>410</v>
+      </c>
+      <c r="D393" t="s">
+        <v>378</v>
+      </c>
+      <c r="E393">
+        <v>43.332479999999997</v>
+      </c>
+      <c r="F393">
+        <v>15.169298545790401</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>462</v>
+      </c>
+      <c r="B394">
+        <v>1</v>
+      </c>
+      <c r="C394" t="s">
+        <v>93</v>
+      </c>
+      <c r="D394" t="s">
+        <v>343</v>
+      </c>
+      <c r="E394">
+        <v>46.7299705</v>
+      </c>
+      <c r="F394">
+        <v>11.575639562657599</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>464</v>
+      </c>
+      <c r="B395">
+        <v>1</v>
+      </c>
+      <c r="C395" t="s">
+        <v>257</v>
+      </c>
+      <c r="D395" t="s">
+        <v>365</v>
+      </c>
+      <c r="E395">
+        <v>46.183089199999998</v>
+      </c>
+      <c r="F395">
+        <v>17.740352654195501</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>473</v>
+      </c>
+      <c r="B396">
+        <v>1</v>
+      </c>
+      <c r="C396" t="s">
+        <v>258</v>
+      </c>
+      <c r="D396" t="s">
+        <v>370</v>
+      </c>
+      <c r="E396">
+        <v>39.210346199999996</v>
+      </c>
+      <c r="F396">
+        <v>9.0446191015954902</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>497</v>
+      </c>
+      <c r="B397">
+        <v>1</v>
+      </c>
+      <c r="C397" t="s">
+        <v>411</v>
+      </c>
+      <c r="D397" t="s">
+        <v>378</v>
+      </c>
+      <c r="E397">
+        <v>46.718313500000001</v>
+      </c>
+      <c r="F397">
+        <v>4.3071068076723504</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>498</v>
+      </c>
+      <c r="B398">
+        <v>1</v>
+      </c>
+      <c r="C398" t="s">
+        <v>100</v>
+      </c>
+      <c r="D398" t="s">
+        <v>343</v>
+      </c>
+      <c r="E398">
+        <v>45.470928200000003</v>
+      </c>
+      <c r="F398">
+        <v>12.925434718766599</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>500</v>
+      </c>
+      <c r="B399">
+        <v>1</v>
+      </c>
+      <c r="C399" t="s">
+        <v>261</v>
+      </c>
+      <c r="D399" t="s">
+        <v>365</v>
+      </c>
+      <c r="E399">
+        <v>43.788561600000001</v>
+      </c>
+      <c r="F399">
+        <v>13.7761100343123</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>501</v>
+      </c>
+      <c r="B400">
+        <v>1</v>
+      </c>
+      <c r="C400" t="s">
+        <v>101</v>
+      </c>
+      <c r="D400" t="s">
+        <v>364</v>
+      </c>
+      <c r="E400">
+        <v>42.559879199999997</v>
+      </c>
+      <c r="F400">
+        <v>25.529310785085499</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>504</v>
+      </c>
+      <c r="B401">
+        <v>-1</v>
+      </c>
+      <c r="C401" t="s">
+        <v>264</v>
+      </c>
+      <c r="D401" t="s">
+        <v>412</v>
+      </c>
+      <c r="E401">
+        <v>67.033795799999993</v>
+      </c>
+      <c r="F401">
+        <v>10.445142150793499</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>509</v>
+      </c>
+      <c r="B402">
+        <v>1</v>
+      </c>
+      <c r="C402" t="s">
+        <v>265</v>
+      </c>
+      <c r="D402" t="s">
+        <v>412</v>
+      </c>
+      <c r="E402">
+        <v>64.864599999999996</v>
+      </c>
+      <c r="F402">
+        <v>13.0199913975635</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>518</v>
+      </c>
+      <c r="B403">
+        <v>-1</v>
+      </c>
+      <c r="C403" t="s">
+        <v>413</v>
+      </c>
+      <c r="D403" t="s">
+        <v>380</v>
+      </c>
+      <c r="E403">
+        <v>45.531536899999999</v>
+      </c>
+      <c r="F403">
+        <v>4.4185273867559101</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>547</v>
+      </c>
+      <c r="B404">
+        <v>-1</v>
+      </c>
+      <c r="C404" t="s">
+        <v>414</v>
+      </c>
+      <c r="D404" t="s">
+        <v>408</v>
+      </c>
+      <c r="E404">
+        <v>43.519672</v>
+      </c>
+      <c r="F404">
+        <v>1.5135353773523299</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>552</v>
+      </c>
+      <c r="B405">
+        <v>1</v>
+      </c>
+      <c r="C405" t="s">
+        <v>415</v>
+      </c>
+      <c r="D405" t="s">
+        <v>340</v>
+      </c>
+      <c r="E405">
+        <v>44.210341499999998</v>
+      </c>
+      <c r="F405">
+        <v>15.062429131428599</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>562</v>
+      </c>
+      <c r="B406">
+        <v>1</v>
+      </c>
+      <c r="C406" t="s">
+        <v>416</v>
+      </c>
+      <c r="D406" t="s">
+        <v>347</v>
+      </c>
+      <c r="E406">
+        <v>43.6921927</v>
+      </c>
+      <c r="F406">
+        <v>22.849395717112699</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>562</v>
+      </c>
+      <c r="B407">
+        <v>-1</v>
+      </c>
+      <c r="C407" t="s">
+        <v>417</v>
+      </c>
+      <c r="D407" t="s">
+        <v>418</v>
+      </c>
+      <c r="E407">
+        <v>38.132736999999999</v>
+      </c>
+      <c r="F407">
+        <v>5.0113966545951296</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>564</v>
+      </c>
+      <c r="B408">
+        <v>1</v>
+      </c>
+      <c r="C408" t="s">
+        <v>274</v>
+      </c>
+      <c r="D408" t="s">
+        <v>338</v>
+      </c>
+      <c r="E408">
+        <v>58.010871999999999</v>
+      </c>
+      <c r="F408">
+        <v>2.53430426445862</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>568</v>
+      </c>
+      <c r="B409">
+        <v>1</v>
+      </c>
+      <c r="C409" t="s">
+        <v>419</v>
+      </c>
+      <c r="D409" t="s">
+        <v>420</v>
+      </c>
+      <c r="E409">
+        <v>70.021821099999997</v>
+      </c>
+      <c r="F409">
+        <v>3.9684347678272198</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>581</v>
+      </c>
+      <c r="B410">
+        <v>1</v>
+      </c>
+      <c r="C410" t="s">
+        <v>421</v>
+      </c>
+      <c r="D410" t="s">
+        <v>422</v>
+      </c>
+      <c r="E410">
+        <v>47.168664</v>
+      </c>
+      <c r="F410">
+        <v>32.410494768149697</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>590</v>
+      </c>
+      <c r="B411">
+        <v>1</v>
+      </c>
+      <c r="C411" t="s">
+        <v>279</v>
+      </c>
+      <c r="D411" t="s">
+        <v>356</v>
+      </c>
+      <c r="E411">
+        <v>42.235273999999997</v>
+      </c>
+      <c r="F411">
+        <v>0.74369283602647196</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>594</v>
+      </c>
+      <c r="B412">
+        <v>1</v>
+      </c>
+      <c r="C412" t="s">
+        <v>423</v>
+      </c>
+      <c r="D412" t="s">
+        <v>424</v>
+      </c>
+      <c r="E412">
+        <v>41.543861499999998</v>
+      </c>
+      <c r="F412">
+        <v>60.762784902928701</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>599</v>
+      </c>
+      <c r="B413">
+        <v>-1</v>
+      </c>
+      <c r="C413" t="s">
+        <v>425</v>
+      </c>
+      <c r="D413" t="s">
+        <v>345</v>
+      </c>
+      <c r="E413">
+        <v>44.082004499999996</v>
+      </c>
+      <c r="F413">
+        <v>23.029328746378599</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>602</v>
+      </c>
+      <c r="B414">
+        <v>1</v>
+      </c>
+      <c r="C414" t="s">
+        <v>281</v>
+      </c>
+      <c r="D414" t="s">
+        <v>349</v>
+      </c>
+      <c r="E414">
+        <v>45.140993799999997</v>
+      </c>
+      <c r="F414">
+        <v>10.3533999618096</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>611</v>
+      </c>
+      <c r="B415">
+        <v>-1</v>
+      </c>
+      <c r="C415" t="s">
+        <v>426</v>
+      </c>
+      <c r="D415" t="s">
+        <v>345</v>
+      </c>
+      <c r="E415">
+        <v>47.382850900000001</v>
+      </c>
+      <c r="F415">
+        <v>30.486490582933801</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>621</v>
+      </c>
+      <c r="B416">
+        <v>1</v>
+      </c>
+      <c r="C416" t="s">
+        <v>427</v>
+      </c>
+      <c r="D416" t="s">
+        <v>422</v>
+      </c>
+      <c r="E416">
+        <v>47.568379700000001</v>
+      </c>
+      <c r="F416">
+        <v>13.952887018882601</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>643</v>
+      </c>
+      <c r="B417">
+        <v>-1</v>
+      </c>
+      <c r="C417" t="s">
+        <v>286</v>
+      </c>
+      <c r="D417" t="s">
+        <v>356</v>
+      </c>
+      <c r="E417">
+        <v>38.008584900000002</v>
+      </c>
+      <c r="F417">
+        <v>3.2665694513161898</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>648</v>
+      </c>
+      <c r="B418">
+        <v>-1</v>
+      </c>
+      <c r="C418" t="s">
+        <v>123</v>
+      </c>
+      <c r="D418" t="s">
+        <v>343</v>
+      </c>
+      <c r="E418">
+        <v>40.748559299999997</v>
+      </c>
+      <c r="F418">
+        <v>10.845278888909</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>649</v>
+      </c>
+      <c r="B419">
+        <v>-1</v>
+      </c>
+      <c r="C419" t="s">
+        <v>428</v>
+      </c>
+      <c r="D419" t="s">
+        <v>378</v>
+      </c>
+      <c r="E419">
+        <v>41.0953175</v>
+      </c>
+      <c r="F419">
+        <v>4.0679223756581697</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>657</v>
+      </c>
+      <c r="B420">
+        <v>-1</v>
+      </c>
+      <c r="C420" t="s">
+        <v>126</v>
+      </c>
+      <c r="D420" t="s">
+        <v>355</v>
+      </c>
+      <c r="E420">
+        <v>38.727040600000002</v>
+      </c>
+      <c r="F420">
+        <v>2.4171951241301799</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>658</v>
+      </c>
+      <c r="B421">
+        <v>-1</v>
+      </c>
+      <c r="C421" t="s">
+        <v>288</v>
+      </c>
+      <c r="D421" t="s">
+        <v>429</v>
+      </c>
+      <c r="E421">
+        <v>37.346784200000002</v>
+      </c>
+      <c r="F421">
+        <v>4.1485549768518499</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>668</v>
+      </c>
+      <c r="B422">
+        <v>1</v>
+      </c>
+      <c r="C422" t="s">
+        <v>290</v>
+      </c>
+      <c r="D422" t="s">
+        <v>370</v>
+      </c>
+      <c r="E422">
+        <v>46.263106000000001</v>
+      </c>
+      <c r="F422">
+        <v>50.367996855150103</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>668</v>
+      </c>
+      <c r="B423">
+        <v>-1</v>
+      </c>
+      <c r="C423" t="s">
+        <v>291</v>
+      </c>
+      <c r="D423" t="s">
+        <v>430</v>
+      </c>
+      <c r="E423">
+        <v>45.507732900000001</v>
+      </c>
+      <c r="F423">
+        <v>1.2434980230319299</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A424">
+        <v>670</v>
+      </c>
+      <c r="B424">
+        <v>-1</v>
+      </c>
+      <c r="C424" t="s">
+        <v>431</v>
+      </c>
+      <c r="D424" t="s">
+        <v>347</v>
+      </c>
+      <c r="E424">
+        <v>45.132940699999999</v>
+      </c>
+      <c r="F424">
+        <v>39.621486389955997</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>675</v>
+      </c>
+      <c r="B425">
+        <v>-1</v>
+      </c>
+      <c r="C425" t="s">
+        <v>432</v>
+      </c>
+      <c r="D425" t="s">
+        <v>372</v>
+      </c>
+      <c r="E425">
+        <v>44.066117900000002</v>
+      </c>
+      <c r="F425">
+        <v>11.1695716381988</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>685</v>
+      </c>
+      <c r="B426">
+        <v>1</v>
+      </c>
+      <c r="C426" t="s">
+        <v>433</v>
+      </c>
+      <c r="D426" t="s">
+        <v>390</v>
+      </c>
+      <c r="E426">
+        <v>46.27702</v>
+      </c>
+      <c r="F426">
+        <v>24.160737045887199</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A427">
+        <v>686</v>
+      </c>
+      <c r="B427">
+        <v>1</v>
+      </c>
+      <c r="C427" t="s">
+        <v>132</v>
+      </c>
+      <c r="D427" t="s">
+        <v>391</v>
+      </c>
+      <c r="E427">
+        <v>44.300574900000001</v>
+      </c>
+      <c r="F427">
+        <v>35.764542180682596</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A428">
+        <v>697</v>
+      </c>
+      <c r="B428">
+        <v>1</v>
+      </c>
+      <c r="C428" t="s">
+        <v>434</v>
+      </c>
+      <c r="D428" t="s">
+        <v>369</v>
+      </c>
+      <c r="E428">
+        <v>79.900725699999995</v>
+      </c>
+      <c r="F428">
+        <v>22.133188641032302</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A429">
+        <v>707</v>
+      </c>
+      <c r="B429">
+        <v>-1</v>
+      </c>
+      <c r="C429" t="s">
+        <v>435</v>
+      </c>
+      <c r="D429" t="s">
+        <v>336</v>
+      </c>
+      <c r="E429">
+        <v>42.000632799999998</v>
+      </c>
+      <c r="F429">
+        <v>6.9143264749632101</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>721</v>
+      </c>
+      <c r="B430">
+        <v>-1</v>
+      </c>
+      <c r="C430" t="s">
+        <v>436</v>
+      </c>
+      <c r="D430" t="s">
+        <v>380</v>
+      </c>
+      <c r="E430">
+        <v>41.568474199999997</v>
+      </c>
+      <c r="F430">
+        <v>50.920232075219701</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>731</v>
+      </c>
+      <c r="B431">
+        <v>1</v>
+      </c>
+      <c r="C431" t="s">
+        <v>298</v>
+      </c>
+      <c r="D431" t="s">
+        <v>370</v>
+      </c>
+      <c r="E431">
+        <v>38.468886099999999</v>
+      </c>
+      <c r="F431">
+        <v>39.775735268176099</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A432">
+        <v>732</v>
+      </c>
+      <c r="B432">
+        <v>1</v>
+      </c>
+      <c r="C432" t="s">
+        <v>141</v>
+      </c>
+      <c r="D432" t="s">
+        <v>364</v>
+      </c>
+      <c r="E432">
+        <v>41.611541899999999</v>
+      </c>
+      <c r="F432">
+        <v>5.7572343745373704</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>734</v>
+      </c>
+      <c r="B433">
+        <v>1</v>
+      </c>
+      <c r="C433" t="s">
+        <v>299</v>
+      </c>
+      <c r="D433" t="s">
+        <v>365</v>
+      </c>
+      <c r="E433">
+        <v>41.349474800000003</v>
+      </c>
+      <c r="F433">
+        <v>69.808253385416805</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A434">
+        <v>735</v>
+      </c>
+      <c r="B434">
+        <v>1</v>
+      </c>
+      <c r="C434" t="s">
+        <v>142</v>
+      </c>
+      <c r="D434" t="s">
+        <v>364</v>
+      </c>
+      <c r="E434">
+        <v>39.495398899999998</v>
+      </c>
+      <c r="F434">
+        <v>38.563695881742802</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A435">
+        <v>759</v>
+      </c>
+      <c r="B435">
+        <v>1</v>
+      </c>
+      <c r="C435" t="s">
+        <v>437</v>
+      </c>
+      <c r="D435" t="s">
+        <v>374</v>
+      </c>
+      <c r="E435">
+        <v>42.551390499999997</v>
+      </c>
+      <c r="F435">
+        <v>15.882493410679601</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A436">
+        <v>761</v>
+      </c>
+      <c r="B436">
+        <v>1</v>
+      </c>
+      <c r="C436" t="s">
+        <v>305</v>
+      </c>
+      <c r="D436" t="s">
+        <v>338</v>
+      </c>
+      <c r="E436">
+        <v>46.995623000000002</v>
+      </c>
+      <c r="F436">
+        <v>10.2378231442074</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A437">
+        <v>778</v>
+      </c>
+      <c r="B437">
+        <v>-1</v>
+      </c>
+      <c r="C437" t="s">
+        <v>148</v>
+      </c>
+      <c r="D437" t="s">
+        <v>337</v>
+      </c>
+      <c r="E437">
+        <v>48.7029402</v>
+      </c>
+      <c r="F437">
+        <v>30.7227744119485</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A438">
+        <v>779</v>
+      </c>
+      <c r="B438">
+        <v>-1</v>
+      </c>
+      <c r="C438" t="s">
+        <v>438</v>
+      </c>
+      <c r="D438" t="s">
+        <v>342</v>
+      </c>
+      <c r="E438">
+        <v>48.542754700000003</v>
+      </c>
+      <c r="F438">
+        <v>20.8228482798465</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A439">
+        <v>797</v>
+      </c>
+      <c r="B439">
+        <v>-1</v>
+      </c>
+      <c r="C439" t="s">
+        <v>439</v>
+      </c>
+      <c r="D439" t="s">
+        <v>380</v>
+      </c>
+      <c r="E439">
+        <v>35.046033299999998</v>
+      </c>
+      <c r="F439">
+        <v>6.8866118676499397</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A440">
+        <v>801</v>
+      </c>
+      <c r="B440">
+        <v>1</v>
+      </c>
+      <c r="C440" t="s">
+        <v>440</v>
+      </c>
+      <c r="D440" t="s">
+        <v>441</v>
+      </c>
+      <c r="E440">
+        <v>41.865909199999997</v>
+      </c>
+      <c r="F440">
+        <v>7.5893889453530603</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A441">
+        <v>808</v>
+      </c>
+      <c r="B441">
+        <v>1</v>
+      </c>
+      <c r="C441" t="s">
+        <v>442</v>
+      </c>
+      <c r="D441" t="s">
+        <v>345</v>
+      </c>
+      <c r="E441">
+        <v>46.241798699999997</v>
+      </c>
+      <c r="F441">
+        <v>1.50880090824776</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A442">
+        <v>817</v>
+      </c>
+      <c r="B442">
+        <v>-1</v>
+      </c>
+      <c r="C442" t="s">
+        <v>311</v>
+      </c>
+      <c r="D442" t="s">
+        <v>356</v>
+      </c>
+      <c r="E442">
+        <v>44.957918399999997</v>
+      </c>
+      <c r="F442">
+        <v>3.2501799120146799</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A443">
+        <v>818</v>
+      </c>
+      <c r="B443">
+        <v>1</v>
+      </c>
+      <c r="C443" t="s">
+        <v>443</v>
+      </c>
+      <c r="D443" t="s">
+        <v>444</v>
+      </c>
+      <c r="E443">
+        <v>43.047514700000001</v>
+      </c>
+      <c r="F443">
+        <v>36.248351918807003</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A444">
+        <v>824</v>
+      </c>
+      <c r="B444">
+        <v>1</v>
+      </c>
+      <c r="C444" t="s">
+        <v>445</v>
+      </c>
+      <c r="D444" t="s">
+        <v>378</v>
+      </c>
+      <c r="E444">
+        <v>45.265175300000003</v>
+      </c>
+      <c r="F444">
+        <v>17.440767498281101</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A445">
+        <v>824</v>
+      </c>
+      <c r="B445">
+        <v>-1</v>
+      </c>
+      <c r="C445" t="s">
+        <v>446</v>
+      </c>
+      <c r="D445" t="s">
+        <v>345</v>
+      </c>
+      <c r="E445">
+        <v>76.788355899999999</v>
+      </c>
+      <c r="F445">
+        <v>4.30707404111019</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A446">
+        <v>825</v>
+      </c>
+      <c r="B446">
+        <v>1</v>
+      </c>
+      <c r="C446" t="s">
+        <v>162</v>
+      </c>
+      <c r="D446" t="s">
+        <v>343</v>
+      </c>
+      <c r="E446">
+        <v>44.322276799999997</v>
+      </c>
+      <c r="F446">
+        <v>4.7120061882129001</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A447">
+        <v>827</v>
+      </c>
+      <c r="B447">
+        <v>1</v>
+      </c>
+      <c r="C447" t="s">
+        <v>313</v>
+      </c>
+      <c r="D447" t="s">
+        <v>365</v>
+      </c>
+      <c r="E447">
+        <v>79.476105599999997</v>
+      </c>
+      <c r="F447">
+        <v>5.4789579455470001</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A448">
+        <v>828</v>
+      </c>
+      <c r="B448">
+        <v>1</v>
+      </c>
+      <c r="C448" t="s">
+        <v>163</v>
+      </c>
+      <c r="D448" t="s">
+        <v>447</v>
+      </c>
+      <c r="E448">
+        <v>74.966186500000006</v>
+      </c>
+      <c r="F448">
+        <v>26.049209817952299</v>
+      </c>
+    </row>
+    <row r="449" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>833</v>
+      </c>
+      <c r="B449">
+        <v>1</v>
+      </c>
+      <c r="C449" t="s">
+        <v>448</v>
+      </c>
+      <c r="D449" t="s">
+        <v>390</v>
+      </c>
+      <c r="E449">
+        <v>47.931562499999998</v>
+      </c>
+      <c r="F449">
+        <v>5.2969735942108596</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>834</v>
+      </c>
+      <c r="B450">
+        <v>1</v>
+      </c>
+      <c r="C450" t="s">
+        <v>164</v>
+      </c>
+      <c r="D450" t="s">
+        <v>449</v>
+      </c>
+      <c r="E450">
+        <v>45.371740299999999</v>
+      </c>
+      <c r="F450">
+        <v>2.38293233247422</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A451">
+        <v>849</v>
+      </c>
+      <c r="B451">
+        <v>1</v>
+      </c>
+      <c r="C451" t="s">
+        <v>316</v>
+      </c>
+      <c r="D451" t="s">
+        <v>356</v>
+      </c>
+      <c r="E451">
+        <v>35.380614799999996</v>
+      </c>
+      <c r="F451">
+        <v>3.5909231191468698</v>
+      </c>
+    </row>
+    <row r="452" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A452">
+        <v>866</v>
+      </c>
+      <c r="B452">
+        <v>1</v>
+      </c>
+      <c r="C452" t="s">
+        <v>450</v>
+      </c>
+      <c r="D452" t="s">
+        <v>345</v>
+      </c>
+      <c r="E452">
+        <v>39.521391199999997</v>
+      </c>
+      <c r="F452">
+        <v>1.98234221784234</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A453">
+        <v>867</v>
+      </c>
+      <c r="B453">
+        <v>1</v>
+      </c>
+      <c r="C453" t="s">
+        <v>172</v>
+      </c>
+      <c r="D453" t="s">
+        <v>343</v>
+      </c>
+      <c r="E453">
+        <v>39.793658499999999</v>
+      </c>
+      <c r="F453">
+        <v>0.57349701788496199</v>
+      </c>
+    </row>
+    <row r="454" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A454">
+        <v>869</v>
+      </c>
+      <c r="B454">
+        <v>1</v>
+      </c>
+      <c r="C454" t="s">
+        <v>321</v>
+      </c>
+      <c r="D454" t="s">
+        <v>365</v>
+      </c>
+      <c r="E454">
+        <v>41.491344400000003</v>
+      </c>
+      <c r="F454">
+        <v>5.50250075242531</v>
+      </c>
+    </row>
+    <row r="455" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A455">
+        <v>870</v>
+      </c>
+      <c r="B455">
+        <v>1</v>
+      </c>
+      <c r="C455" t="s">
+        <v>173</v>
+      </c>
+      <c r="D455" t="s">
+        <v>364</v>
+      </c>
+      <c r="E455">
+        <v>42.780695700000003</v>
+      </c>
+      <c r="F455">
+        <v>13.5260227095115</v>
+      </c>
+    </row>
+    <row r="456" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>873</v>
+      </c>
+      <c r="B456">
+        <v>-1</v>
+      </c>
+      <c r="C456" t="s">
+        <v>324</v>
+      </c>
+      <c r="D456" t="s">
+        <v>338</v>
+      </c>
+      <c r="E456">
+        <v>36.069175799999996</v>
+      </c>
+      <c r="F456">
+        <v>19.3359186715366</v>
+      </c>
+    </row>
+    <row r="457" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A457">
+        <v>875</v>
+      </c>
+      <c r="B457">
+        <v>-1</v>
+      </c>
+      <c r="C457" t="s">
+        <v>326</v>
+      </c>
+      <c r="D457" t="s">
+        <v>412</v>
+      </c>
+      <c r="E457">
+        <v>37.553134700000001</v>
+      </c>
+      <c r="F457">
+        <v>1.4655740072907</v>
+      </c>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A458">
+        <v>882</v>
+      </c>
+      <c r="B458">
+        <v>1</v>
+      </c>
+      <c r="C458" t="s">
+        <v>451</v>
+      </c>
+      <c r="D458" t="s">
+        <v>380</v>
+      </c>
+      <c r="E458">
+        <v>34.258759699999999</v>
+      </c>
+      <c r="F458">
+        <v>14.5261310998666</v>
+      </c>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A459">
+        <v>896</v>
+      </c>
+      <c r="B459">
+        <v>1</v>
+      </c>
+      <c r="C459" t="s">
+        <v>329</v>
+      </c>
+      <c r="D459" t="s">
+        <v>370</v>
+      </c>
+      <c r="E459">
+        <v>45.576647700000002</v>
+      </c>
+      <c r="F459">
+        <v>33.634009309145803</v>
+      </c>
+    </row>
+    <row r="460" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A460">
+        <v>897</v>
+      </c>
+      <c r="B460">
+        <v>1</v>
+      </c>
+      <c r="C460" t="s">
+        <v>178</v>
+      </c>
+      <c r="D460" t="s">
+        <v>364</v>
+      </c>
+      <c r="E460">
+        <v>46.306840899999997</v>
+      </c>
+      <c r="F460">
+        <v>0.70954449487828197</v>
+      </c>
+    </row>
+    <row r="461" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A461">
+        <v>902</v>
+      </c>
+      <c r="B461">
+        <v>1</v>
+      </c>
+      <c r="C461" t="s">
+        <v>331</v>
+      </c>
+      <c r="D461" t="s">
+        <v>349</v>
+      </c>
+      <c r="E461">
+        <v>33.735238699999996</v>
+      </c>
+      <c r="F461">
+        <v>6.5154925906189201</v>
+      </c>
+    </row>
+    <row r="462" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A462">
+        <v>44</v>
+      </c>
+      <c r="B462">
+        <v>-1</v>
+      </c>
+      <c r="C462" t="s">
+        <v>341</v>
+      </c>
+      <c r="D462" t="s">
+        <v>452</v>
+      </c>
+      <c r="E462">
+        <v>41.2558705</v>
+      </c>
+      <c r="F462">
+        <v>7.03561876758664</v>
+      </c>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A463">
+        <v>61</v>
+      </c>
+      <c r="B463">
+        <v>-1</v>
+      </c>
+      <c r="C463" t="s">
+        <v>14</v>
+      </c>
+      <c r="D463" t="s">
+        <v>453</v>
+      </c>
+      <c r="E463">
+        <v>41.119681399999997</v>
+      </c>
+      <c r="F463">
+        <v>16.570492504943498</v>
+      </c>
+    </row>
+    <row r="464" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A464">
+        <v>116</v>
+      </c>
+      <c r="B464">
+        <v>-1</v>
+      </c>
+      <c r="C464" t="s">
+        <v>366</v>
+      </c>
+      <c r="D464" t="s">
+        <v>454</v>
+      </c>
+      <c r="E464">
+        <v>54.2540993</v>
+      </c>
+      <c r="F464">
+        <v>1.82591648618067</v>
+      </c>
+    </row>
+    <row r="465" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A465">
+        <v>156</v>
+      </c>
+      <c r="B465">
+        <v>-1</v>
+      </c>
+      <c r="C465" t="s">
+        <v>368</v>
+      </c>
+      <c r="D465" t="s">
+        <v>455</v>
+      </c>
+      <c r="E465">
+        <v>45.188416199999999</v>
+      </c>
+      <c r="F465">
+        <v>67.486109203991106</v>
+      </c>
+    </row>
+    <row r="466" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A466">
+        <v>290</v>
+      </c>
+      <c r="B466">
+        <v>1</v>
+      </c>
+      <c r="C466" t="s">
+        <v>386</v>
+      </c>
+      <c r="D466" t="s">
+        <v>456</v>
+      </c>
+      <c r="E466">
+        <v>45.078523400000002</v>
+      </c>
+      <c r="F466">
+        <v>54.976586001604403</v>
+      </c>
+    </row>
+    <row r="467" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A467">
+        <v>350</v>
+      </c>
+      <c r="B467">
+        <v>-1</v>
+      </c>
+      <c r="C467" t="s">
+        <v>241</v>
+      </c>
+      <c r="D467" t="s">
+        <v>457</v>
+      </c>
+      <c r="E467">
+        <v>44.425019300000002</v>
+      </c>
+      <c r="F467">
+        <v>16.613114018256599</v>
+      </c>
+    </row>
+    <row r="468" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A468">
+        <v>356</v>
+      </c>
+      <c r="B468">
+        <v>1</v>
+      </c>
+      <c r="C468" t="s">
+        <v>72</v>
+      </c>
+      <c r="D468" t="s">
+        <v>458</v>
+      </c>
+      <c r="E468">
+        <v>37.103979199999998</v>
+      </c>
+      <c r="F468">
+        <v>49.076943134890001</v>
+      </c>
+    </row>
+    <row r="469" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A469">
+        <v>356</v>
+      </c>
+      <c r="B469">
+        <v>-1</v>
+      </c>
+      <c r="C469" t="s">
+        <v>396</v>
+      </c>
+      <c r="D469" t="s">
+        <v>459</v>
+      </c>
+      <c r="E469">
+        <v>96.029895400000001</v>
+      </c>
+      <c r="F469">
+        <v>5.89317389925833</v>
+      </c>
+    </row>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A470">
+        <v>370</v>
+      </c>
+      <c r="B470">
+        <v>1</v>
+      </c>
+      <c r="C470" t="s">
+        <v>398</v>
+      </c>
+      <c r="D470" t="s">
+        <v>460</v>
+      </c>
+      <c r="E470">
+        <v>94.668598000000003</v>
+      </c>
+      <c r="F470">
+        <v>8.6555626656087892</v>
+      </c>
+    </row>
+    <row r="471" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A471">
+        <v>411</v>
+      </c>
+      <c r="B471">
+        <v>1</v>
+      </c>
+      <c r="C471" t="s">
+        <v>81</v>
+      </c>
+      <c r="D471" t="s">
+        <v>453</v>
+      </c>
+      <c r="E471">
+        <v>48.848190700000004</v>
+      </c>
+      <c r="F471">
+        <v>6.0554803872304097</v>
+      </c>
+    </row>
+    <row r="472" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A472">
+        <v>449</v>
+      </c>
+      <c r="B472">
+        <v>1</v>
+      </c>
+      <c r="C472" t="s">
+        <v>409</v>
+      </c>
+      <c r="D472" t="s">
+        <v>461</v>
+      </c>
+      <c r="E472">
+        <v>44.7592894</v>
+      </c>
+      <c r="F472">
+        <v>25.1359953446722</v>
+      </c>
+    </row>
+    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A473">
+        <v>504</v>
+      </c>
+      <c r="B473">
+        <v>-1</v>
+      </c>
+      <c r="C473" t="s">
+        <v>264</v>
+      </c>
+      <c r="D473" t="s">
+        <v>462</v>
+      </c>
+      <c r="E473">
+        <v>67.033795799999993</v>
+      </c>
+      <c r="F473">
+        <v>10.445142150793499</v>
+      </c>
+    </row>
+    <row r="474" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A474">
+        <v>518</v>
+      </c>
+      <c r="B474">
+        <v>-1</v>
+      </c>
+      <c r="C474" t="s">
+        <v>413</v>
+      </c>
+      <c r="D474" t="s">
+        <v>459</v>
+      </c>
+      <c r="E474">
+        <v>45.531536899999999</v>
+      </c>
+      <c r="F474">
+        <v>4.4185273867559101</v>
+      </c>
+    </row>
+    <row r="475" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A475">
+        <v>590</v>
+      </c>
+      <c r="B475">
+        <v>1</v>
+      </c>
+      <c r="C475" t="s">
+        <v>279</v>
+      </c>
+      <c r="D475" t="s">
+        <v>457</v>
+      </c>
+      <c r="E475">
+        <v>42.235273999999997</v>
+      </c>
+      <c r="F475">
+        <v>0.74369283602647196</v>
+      </c>
+    </row>
+    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A476">
+        <v>599</v>
+      </c>
+      <c r="B476">
+        <v>-1</v>
+      </c>
+      <c r="C476" t="s">
+        <v>425</v>
+      </c>
+      <c r="D476" t="s">
+        <v>461</v>
+      </c>
+      <c r="E476">
+        <v>44.082004499999996</v>
+      </c>
+      <c r="F476">
+        <v>23.029328746378599</v>
+      </c>
+    </row>
+    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A477">
+        <v>611</v>
+      </c>
+      <c r="B477">
+        <v>-1</v>
+      </c>
+      <c r="C477" t="s">
+        <v>426</v>
+      </c>
+      <c r="D477" t="s">
+        <v>461</v>
+      </c>
+      <c r="E477">
+        <v>47.382850900000001</v>
+      </c>
+      <c r="F477">
+        <v>30.486490582933801</v>
+      </c>
+    </row>
+    <row r="478" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A478">
+        <v>657</v>
+      </c>
+      <c r="B478">
+        <v>-1</v>
+      </c>
+      <c r="C478" t="s">
+        <v>126</v>
+      </c>
+      <c r="D478" t="s">
+        <v>463</v>
+      </c>
+      <c r="E478">
+        <v>38.727040600000002</v>
+      </c>
+      <c r="F478">
+        <v>2.4171951241301799</v>
+      </c>
+    </row>
+    <row r="479" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A479">
+        <v>668</v>
+      </c>
+      <c r="B479">
+        <v>-1</v>
+      </c>
+      <c r="C479" t="s">
+        <v>291</v>
+      </c>
+      <c r="D479" t="s">
+        <v>464</v>
+      </c>
+      <c r="E479">
+        <v>45.507732900000001</v>
+      </c>
+      <c r="F479">
+        <v>1.2434980230319299</v>
+      </c>
+    </row>
+    <row r="480" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A480">
+        <v>686</v>
+      </c>
+      <c r="B480">
+        <v>1</v>
+      </c>
+      <c r="C480" t="s">
+        <v>132</v>
+      </c>
+      <c r="D480" t="s">
+        <v>465</v>
+      </c>
+      <c r="E480">
+        <v>44.300574900000001</v>
+      </c>
+      <c r="F480">
+        <v>35.764542180682596</v>
+      </c>
+    </row>
+    <row r="481" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A481">
+        <v>808</v>
+      </c>
+      <c r="B481">
+        <v>1</v>
+      </c>
+      <c r="C481" t="s">
+        <v>442</v>
+      </c>
+      <c r="D481" t="s">
+        <v>461</v>
+      </c>
+      <c r="E481">
+        <v>46.241798699999997</v>
+      </c>
+      <c r="F481">
+        <v>1.50880090824776</v>
+      </c>
+    </row>
+    <row r="482" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A482">
+        <v>817</v>
+      </c>
+      <c r="B482">
+        <v>-1</v>
+      </c>
+      <c r="C482" t="s">
+        <v>311</v>
+      </c>
+      <c r="D482" t="s">
+        <v>457</v>
+      </c>
+      <c r="E482">
+        <v>44.957918399999997</v>
+      </c>
+      <c r="F482">
+        <v>3.2501799120146799</v>
+      </c>
+    </row>
+    <row r="483" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A483">
+        <v>824</v>
+      </c>
+      <c r="B483">
+        <v>-1</v>
+      </c>
+      <c r="C483" t="s">
+        <v>446</v>
+      </c>
+      <c r="D483" t="s">
+        <v>461</v>
+      </c>
+      <c r="E483">
+        <v>76.788355899999999</v>
+      </c>
+      <c r="F483">
+        <v>4.30707404111019</v>
+      </c>
+    </row>
+    <row r="484" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A484">
+        <v>95</v>
+      </c>
+      <c r="B484">
+        <v>-1</v>
+      </c>
+      <c r="C484" t="s">
+        <v>22</v>
+      </c>
+      <c r="D484" t="s">
+        <v>466</v>
+      </c>
+      <c r="E484">
+        <v>98.079066600000004</v>
+      </c>
+    </row>
+    <row r="485" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A485">
+        <v>177</v>
+      </c>
+      <c r="B485">
+        <v>1</v>
+      </c>
+      <c r="C485" t="s">
+        <v>467</v>
+      </c>
+      <c r="D485" t="s">
+        <v>468</v>
+      </c>
+      <c r="E485">
+        <v>49.802621100000003</v>
+      </c>
+    </row>
+    <row r="486" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A486">
+        <v>220</v>
+      </c>
+      <c r="B486">
+        <v>1</v>
+      </c>
+      <c r="C486" t="s">
+        <v>220</v>
+      </c>
+      <c r="D486" t="s">
+        <v>468</v>
+      </c>
+      <c r="E486">
+        <v>49.822202599999997</v>
+      </c>
+    </row>
+    <row r="487" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A487">
+        <v>442</v>
+      </c>
+      <c r="B487">
+        <v>1</v>
+      </c>
+      <c r="C487" t="s">
+        <v>469</v>
+      </c>
+      <c r="D487" t="s">
+        <v>468</v>
+      </c>
+      <c r="E487">
+        <v>49.874434399999998</v>
+      </c>
+    </row>
+    <row r="488" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A488">
+        <v>683</v>
+      </c>
+      <c r="B488">
+        <v>-1</v>
+      </c>
+      <c r="C488" t="s">
+        <v>470</v>
+      </c>
+      <c r="D488" t="s">
+        <v>466</v>
+      </c>
+      <c r="E488">
+        <v>98.108204799999996</v>
+      </c>
+    </row>
+    <row r="489" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A489">
+        <v>740</v>
+      </c>
+      <c r="B489">
+        <v>-1</v>
+      </c>
+      <c r="C489" t="s">
+        <v>471</v>
+      </c>
+      <c r="D489" t="s">
+        <v>472</v>
+      </c>
+      <c r="E489">
+        <v>48.650184099999997</v>
+      </c>
+    </row>
+    <row r="490" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A490">
+        <v>805</v>
+      </c>
+      <c r="B490">
+        <v>1</v>
+      </c>
+      <c r="C490" t="s">
+        <v>473</v>
+      </c>
+      <c r="D490" t="s">
+        <v>468</v>
+      </c>
+      <c r="E490">
+        <v>48.700757199999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>